<commit_message>
filter by semester year
</commit_message>
<xml_diff>
--- a/temp/file.xlsx
+++ b/temp/file.xlsx
@@ -15,9 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="193">
-  <si>
-    <t>รายชื่อนักศึกษาที่ลงทะเบียนเรียน ภาคเรียนที่ 2 ปีการศึกษา 2557</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="278">
+  <si>
+    <t>รายชื่อนักศึกษาที่ลงทะเบียนเรียน ภาคเรียนที่ 1 ปีการศึกษา 2557</t>
   </si>
   <si>
     <t xml:space="preserve">  COURSE NO :</t>
@@ -29,7 +29,7 @@
     <t xml:space="preserve">  TITLE :</t>
   </si>
   <si>
-    <t xml:space="preserve">                 IT AND MODERN LIFE                                </t>
+    <t xml:space="preserve">                 IT AND MODERN LIFE</t>
   </si>
   <si>
     <t xml:space="preserve">  SECTION (lec/lab) :</t>
@@ -41,7 +41,7 @@
     <t xml:space="preserve">  LECTURER :</t>
   </si>
   <si>
-    <t xml:space="preserve">                 กิตติพิชญ์   คุปตะวาณิช</t>
+    <t xml:space="preserve">                 วาสนา   นัยโพธิ์</t>
   </si>
   <si>
     <t xml:space="preserve">  DATE :</t>
@@ -59,541 +59,796 @@
     <t>ชื่อ - นามสกุล</t>
   </si>
   <si>
-    <t>นายพงศธร</t>
-  </si>
-  <si>
-    <t>คิดถี</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                               W                                  </t>
-  </si>
-  <si>
-    <t>นางสาวภัทรพรรณ</t>
-  </si>
-  <si>
-    <t>เพียนอก</t>
+    <t>นางสาวกิตติยา</t>
+  </si>
+  <si>
+    <t>พูลอุดม</t>
   </si>
   <si>
     <t xml:space="preserve">                                                                 </t>
   </si>
   <si>
-    <t>นางสาวรุจี</t>
-  </si>
-  <si>
-    <t>ต้นเหลือง</t>
-  </si>
-  <si>
-    <t>นายพงศ์ภัค</t>
-  </si>
-  <si>
-    <t>ประภากรมณฑล</t>
-  </si>
-  <si>
-    <t>นางสาวจริยา</t>
-  </si>
-  <si>
-    <t>สุขเเก้ว</t>
-  </si>
-  <si>
-    <t>นางสาวนภาพร</t>
-  </si>
-  <si>
-    <t>แก้วแสงทอง</t>
-  </si>
-  <si>
-    <t>นางสาวสุทธิดา</t>
-  </si>
-  <si>
-    <t>กันธิมา</t>
+    <t>นางสาวชลลัดดา</t>
+  </si>
+  <si>
+    <t>วิริยะชินการ</t>
+  </si>
+  <si>
+    <t>นายนพดนัย</t>
+  </si>
+  <si>
+    <t>สมโน</t>
+  </si>
+  <si>
+    <t>นายอคิราภ์</t>
+  </si>
+  <si>
+    <t>ถมยา</t>
+  </si>
+  <si>
+    <t>นางสาวขวัญฤดี</t>
+  </si>
+  <si>
+    <t>มูลวิจิตร์</t>
+  </si>
+  <si>
+    <t>นางสาวฐิติกา</t>
+  </si>
+  <si>
+    <t>ชัยคำรงค์กุล</t>
+  </si>
+  <si>
+    <t>นางสาวปรินดา</t>
+  </si>
+  <si>
+    <t>บุญชุ่ม</t>
+  </si>
+  <si>
+    <t>นางสาวแสงตะวัน</t>
+  </si>
+  <si>
+    <t>วิริยะประสิทธิ์</t>
+  </si>
+  <si>
+    <t>นางสาวพิชญาภา</t>
+  </si>
+  <si>
+    <t>เทพหัสดิน ณ อยุธยา</t>
+  </si>
+  <si>
+    <t>นางสาวพิม</t>
+  </si>
+  <si>
+    <t>สืบแสง</t>
+  </si>
+  <si>
+    <t>นางสาวเพ็ญพิชชา</t>
+  </si>
+  <si>
+    <t>ชุมภูแก้ว</t>
+  </si>
+  <si>
+    <t>นางสาวญาณนันท์</t>
+  </si>
+  <si>
+    <t>ธนีสัตย์</t>
+  </si>
+  <si>
+    <t>นายปรีชาพงษ์</t>
+  </si>
+  <si>
+    <t>นิลแสงสัก</t>
+  </si>
+  <si>
+    <t>นางสาวกฤษณา</t>
+  </si>
+  <si>
+    <t>อุดทารุณ</t>
+  </si>
+  <si>
+    <t>นายจิรัฎฐ์</t>
+  </si>
+  <si>
+    <t>อ่อนแก้ว</t>
+  </si>
+  <si>
+    <t>นางสาวเจตนิพิฐ</t>
+  </si>
+  <si>
+    <t>ดาสินธุ</t>
+  </si>
+  <si>
+    <t>นางสาวบงกชกร</t>
+  </si>
+  <si>
+    <t>ชอบธรรม</t>
+  </si>
+  <si>
+    <t>นางสาวปิยะภรณ์</t>
+  </si>
+  <si>
+    <t>สิงห์ใส</t>
+  </si>
+  <si>
+    <t>นางสาวพิชญ์จิรา</t>
+  </si>
+  <si>
+    <t>ยาอินทร์</t>
+  </si>
+  <si>
+    <t>นางสาวเพ็ญสุภาภรณ์</t>
+  </si>
+  <si>
+    <t>ไตรยศ</t>
+  </si>
+  <si>
+    <t>นางสาวรื่นฤดี</t>
+  </si>
+  <si>
+    <t>คำดี</t>
+  </si>
+  <si>
+    <t>นางสาววรวลัญช์</t>
+  </si>
+  <si>
+    <t>ธิป่าหนาด</t>
+  </si>
+  <si>
+    <t>นางสาววรัญพัชร์</t>
+  </si>
+  <si>
+    <t>จิราสภาพันธ์</t>
+  </si>
+  <si>
+    <t>นางสาวศิรินันท์</t>
+  </si>
+  <si>
+    <t>คำภักดี</t>
+  </si>
+  <si>
+    <t>นางสาวสุดารัตน์</t>
+  </si>
+  <si>
+    <t>ปีหลวง</t>
+  </si>
+  <si>
+    <t>นางสาวอรวี</t>
+  </si>
+  <si>
+    <t>เลาะหะนะ</t>
+  </si>
+  <si>
+    <t>นางสาวฐิตาพร</t>
+  </si>
+  <si>
+    <t>เทียมเจริญ</t>
+  </si>
+  <si>
+    <t>นางสาวฐิติพร</t>
+  </si>
+  <si>
+    <t>ใหม่ชุ่ม</t>
+  </si>
+  <si>
+    <t>นางสาวพฤกษ์สร</t>
+  </si>
+  <si>
+    <t>เสริมกิจ</t>
+  </si>
+  <si>
+    <t>นางสาวพิมพิสุทธิ์</t>
+  </si>
+  <si>
+    <t>อินแปง</t>
+  </si>
+  <si>
+    <t>นางสาววัชราภรณ์</t>
+  </si>
+  <si>
+    <t>ไชยนาม</t>
+  </si>
+  <si>
+    <t>นายกฤษณพงศ์</t>
+  </si>
+  <si>
+    <t>ศรีวงศ์ราช</t>
+  </si>
+  <si>
+    <t>นางสาวเกศราภรณ์</t>
+  </si>
+  <si>
+    <t>ตันสร้าง</t>
+  </si>
+  <si>
+    <t>นางสาวฐิติชญา</t>
+  </si>
+  <si>
+    <t>ฟองอาภา</t>
+  </si>
+  <si>
+    <t>นางสาวธัญญ์นภัส</t>
+  </si>
+  <si>
+    <t>รัฐอริยธำรงค์</t>
+  </si>
+  <si>
+    <t>นางสาวพรจรัส</t>
+  </si>
+  <si>
+    <t>ดีทอง</t>
+  </si>
+  <si>
+    <t>นางสาวพิชชาพร</t>
+  </si>
+  <si>
+    <t>ทิพเนตร</t>
+  </si>
+  <si>
+    <t>นายสรสิช</t>
+  </si>
+  <si>
+    <t>เรืองรุ่ง</t>
+  </si>
+  <si>
+    <t>นายสรายุทธ</t>
+  </si>
+  <si>
+    <t>จรัสพันธุ์กุล</t>
+  </si>
+  <si>
+    <t>นางสาวสิริมา</t>
+  </si>
+  <si>
+    <t>เล้าอติมาน</t>
+  </si>
+  <si>
+    <t>นางสาวสุพรรณษา</t>
+  </si>
+  <si>
+    <t>ยะใจมั่น</t>
+  </si>
+  <si>
+    <t>นางสาวอธิติยา</t>
+  </si>
+  <si>
+    <t>วณะเจริญ</t>
+  </si>
+  <si>
+    <t>นายอรรถวิทย์</t>
+  </si>
+  <si>
+    <t>ศรีสุวรรณ</t>
+  </si>
+  <si>
+    <t>นายอัชเชวะ</t>
+  </si>
+  <si>
+    <t>ชุ่มวงศ์</t>
+  </si>
+  <si>
+    <t>นางสาวอาภาภรณ์</t>
+  </si>
+  <si>
+    <t>พรหมพิงค์</t>
+  </si>
+  <si>
+    <t>นางสาวณัฐพร</t>
+  </si>
+  <si>
+    <t>แก้วพิมล</t>
+  </si>
+  <si>
+    <t>นางสาวอารีย์</t>
+  </si>
+  <si>
+    <t>แสนคำ</t>
+  </si>
+  <si>
+    <t>นายปวริศร์</t>
+  </si>
+  <si>
+    <t>ปิงเมือง</t>
+  </si>
+  <si>
+    <t>นายก้องนเรนทร์</t>
+  </si>
+  <si>
+    <t>ใจคำปัน</t>
+  </si>
+  <si>
+    <t>นางสาวดบัสวินี</t>
+  </si>
+  <si>
+    <t>พุฒโต</t>
+  </si>
+  <si>
+    <t>นางสาวรุ่งนภา</t>
+  </si>
+  <si>
+    <t>ขัติยะราช</t>
+  </si>
+  <si>
+    <t>นายวริทธิ์ธร</t>
+  </si>
+  <si>
+    <t>มอญเพ็ชร</t>
+  </si>
+  <si>
+    <t>พัทมี</t>
+  </si>
+  <si>
+    <t>นางสาวสุภาณี</t>
+  </si>
+  <si>
+    <t>คำนวล</t>
+  </si>
+  <si>
+    <t>นายอนุชิต</t>
+  </si>
+  <si>
+    <t>ลือโฮ้ง</t>
+  </si>
+  <si>
+    <t>นางสาวกฤติยา</t>
+  </si>
+  <si>
+    <t>วงไพวรรณ</t>
+  </si>
+  <si>
+    <t>นายกวีฉัตร</t>
+  </si>
+  <si>
+    <t>วังสาร</t>
+  </si>
+  <si>
+    <t>นางสาวกาญจนา</t>
+  </si>
+  <si>
+    <t>ถานันใจ</t>
+  </si>
+  <si>
+    <t>นายฆนากร</t>
+  </si>
+  <si>
+    <t>จักรใจวงค์</t>
+  </si>
+  <si>
+    <t>นายธนภัทร</t>
+  </si>
+  <si>
+    <t>แสงเขื่อนแก้ว</t>
+  </si>
+  <si>
+    <t>นางสาวบุณยานุช</t>
+  </si>
+  <si>
+    <t>พงษ์มนตรี</t>
+  </si>
+  <si>
+    <t>นางสาวบุษกล</t>
+  </si>
+  <si>
+    <t>กันต์กวี</t>
+  </si>
+  <si>
+    <t>นางสาวสุภาพร</t>
+  </si>
+  <si>
+    <t>ยิ้มสวัสดิ์</t>
+  </si>
+  <si>
+    <t>นางสาวสุภาวดี</t>
+  </si>
+  <si>
+    <t>ศรีใจปัน</t>
+  </si>
+  <si>
+    <t>นางสาวสุวนันท์</t>
+  </si>
+  <si>
+    <t>ลาวเปียง</t>
+  </si>
+  <si>
+    <t>นางสาวสุวรรณี</t>
+  </si>
+  <si>
+    <t>รัตนะ</t>
+  </si>
+  <si>
+    <t>นางสาวสุวิมล</t>
+  </si>
+  <si>
+    <t>อินกูล</t>
+  </si>
+  <si>
+    <t>นายอดิศักดิ์</t>
+  </si>
+  <si>
+    <t>บุญเรือน</t>
+  </si>
+  <si>
+    <t>นายอนันตชัย</t>
+  </si>
+  <si>
+    <t>มูลเจริญขจร</t>
+  </si>
+  <si>
+    <t>นายกรณ์ธนัตถ์</t>
+  </si>
+  <si>
+    <t>สมรรถสินวณิช</t>
+  </si>
+  <si>
+    <t>นางสาวญาสุมินทร์</t>
+  </si>
+  <si>
+    <t>อินทนาคม</t>
+  </si>
+  <si>
+    <t>นางสาวณัฐชา</t>
+  </si>
+  <si>
+    <t>จาตุรพจน์</t>
+  </si>
+  <si>
+    <t>นายพชร</t>
+  </si>
+  <si>
+    <t>พรนิมิตร</t>
+  </si>
+  <si>
+    <t>นางสาวพัณณ์ชิตา</t>
+  </si>
+  <si>
+    <t>คำใส</t>
+  </si>
+  <si>
+    <t>นางสาวพิชญ์สินี</t>
+  </si>
+  <si>
+    <t>สินอยู่</t>
+  </si>
+  <si>
+    <t>นางสาวสโรชาพัชร์</t>
+  </si>
+  <si>
+    <t>บุณยะโสรัจจ์</t>
+  </si>
+  <si>
+    <t>นางสาวสิรดา</t>
+  </si>
+  <si>
+    <t>เดชวงค์ญา</t>
+  </si>
+  <si>
+    <t>นางสาวหทัยชนก</t>
+  </si>
+  <si>
+    <t>ใจกล้า</t>
+  </si>
+  <si>
+    <t>นางสาวอริสรา</t>
+  </si>
+  <si>
+    <t>ชูเชิญ</t>
+  </si>
+  <si>
+    <t>นางสาวกรรณิการ์</t>
+  </si>
+  <si>
+    <t>คำวงษา</t>
+  </si>
+  <si>
+    <t>นางสาวกฤติยากรณ์</t>
+  </si>
+  <si>
+    <t>มะโนเกตุ</t>
+  </si>
+  <si>
+    <t>นางสาวกาญจนาพร</t>
+  </si>
+  <si>
+    <t>แสงสุข</t>
+  </si>
+  <si>
+    <t>นางสาวกุลฉัตร</t>
+  </si>
+  <si>
+    <t>เลิศวิลัย</t>
   </si>
   <si>
     <t>นางสาวกุลธิดา</t>
   </si>
   <si>
-    <t>พุทธเจริญ</t>
-  </si>
-  <si>
-    <t>นายชิษณุพงศ์</t>
-  </si>
-  <si>
-    <t>หาวา</t>
-  </si>
-  <si>
-    <t>นางสาวณิชมน</t>
-  </si>
-  <si>
-    <t>ทองริด</t>
-  </si>
-  <si>
-    <t>นางสาวอภิสรา</t>
-  </si>
-  <si>
-    <t>ฉายาพงศ์</t>
-  </si>
-  <si>
-    <t>นางสาวพิชญา</t>
-  </si>
-  <si>
-    <t>วัชโรภาส</t>
-  </si>
-  <si>
-    <t>นางสาวชนันธิดา</t>
-  </si>
-  <si>
-    <t>สักลอ</t>
-  </si>
-  <si>
-    <t>นางสาวบุญญรัตน์</t>
-  </si>
-  <si>
-    <t>นิวาศะบุตร</t>
-  </si>
-  <si>
-    <t>นางสาวมีณมาส</t>
-  </si>
-  <si>
-    <t>แก่นดี</t>
-  </si>
-  <si>
-    <t>นางสาวกันยา</t>
-  </si>
-  <si>
-    <t>ผาด่าน</t>
-  </si>
-  <si>
-    <t>นายคเชน</t>
-  </si>
-  <si>
-    <t>ศรีวิชัย</t>
-  </si>
-  <si>
-    <t>นายชนสรณ์</t>
-  </si>
-  <si>
-    <t>ศรีสัตบุตร</t>
-  </si>
-  <si>
-    <t>นายคามิน</t>
-  </si>
-  <si>
-    <t>ช่วงสุวนิช</t>
-  </si>
-  <si>
-    <t>นายจุลธวัช</t>
-  </si>
-  <si>
-    <t>ทองอร่าม</t>
-  </si>
-  <si>
-    <t>นายชานนท์</t>
-  </si>
-  <si>
-    <t>ทองมณี</t>
-  </si>
-  <si>
-    <t>นายณัฐดนัย</t>
-  </si>
-  <si>
-    <t>สุขแก้ว</t>
-  </si>
-  <si>
-    <t>นายวรพันธ์</t>
-  </si>
-  <si>
-    <t>คำภู</t>
-  </si>
-  <si>
-    <t>นายสหรัฐ</t>
-  </si>
-  <si>
-    <t>สิทธิปัญญา</t>
-  </si>
-  <si>
-    <t>นางสาวฉัตรชาริกา</t>
-  </si>
-  <si>
-    <t>ขันแก้ว</t>
-  </si>
-  <si>
-    <t>นายเชษฐภัค</t>
-  </si>
-  <si>
-    <t>เรืองดิษฐ์</t>
-  </si>
-  <si>
-    <t>นางสาวธมณภัทร</t>
-  </si>
-  <si>
-    <t>พิทักษ์</t>
-  </si>
-  <si>
-    <t>นางสาวสุนิศา</t>
-  </si>
-  <si>
-    <t>จิ๋วปัญญา</t>
-  </si>
-  <si>
-    <t>นางสาวอนงค์พร</t>
-  </si>
-  <si>
-    <t>เทพสุวรรณ</t>
-  </si>
-  <si>
-    <t>นางสาวอนุตรา</t>
-  </si>
-  <si>
-    <t>ปัญจรัก</t>
-  </si>
-  <si>
-    <t>นางสาวอภิญญา</t>
-  </si>
-  <si>
-    <t>ปานศิลา</t>
-  </si>
-  <si>
-    <t>นายอมรเทพ</t>
-  </si>
-  <si>
-    <t>พิชัยพงศ์</t>
-  </si>
-  <si>
-    <t>นางสาวอมลพรรษ</t>
-  </si>
-  <si>
-    <t>ชตาเริกษ์</t>
-  </si>
-  <si>
-    <t>นางสาวอาภัสนันท์</t>
-  </si>
-  <si>
-    <t>อารีเอื้อ</t>
-  </si>
-  <si>
-    <t>นายเอกภพ</t>
-  </si>
-  <si>
-    <t>พจนสิทธิ์</t>
-  </si>
-  <si>
-    <t>นางสาวศัสยมน</t>
-  </si>
-  <si>
-    <t>ดวงใจสัก</t>
-  </si>
-  <si>
-    <t>นางสาวศุภรัสมิ์</t>
-  </si>
-  <si>
-    <t>กระพันพงศ์สกุล</t>
-  </si>
-  <si>
-    <t>นางสาวศุภวรรณ</t>
-  </si>
-  <si>
-    <t>บุญสุข</t>
-  </si>
-  <si>
-    <t>นายคริษฐ์</t>
-  </si>
-  <si>
-    <t>นิ่มศิริเรืองผล</t>
-  </si>
-  <si>
-    <t>นางสาวจริยาพร</t>
-  </si>
-  <si>
-    <t>จิรพัฒนากุล</t>
-  </si>
-  <si>
-    <t>นางสาวจารุวรรณ</t>
-  </si>
-  <si>
-    <t>โท๊ะหล้าบุตร</t>
-  </si>
-  <si>
-    <t>นายชญาพัฒณ์</t>
-  </si>
-  <si>
-    <t>ภู่เกตุ</t>
-  </si>
-  <si>
-    <t>นางสาวชนนิกานต์</t>
-  </si>
-  <si>
-    <t>เทียนสมจิตร</t>
-  </si>
-  <si>
-    <t>นางสาวชลิดา</t>
-  </si>
-  <si>
-    <t>มานะกิจศิริสุทธิ</t>
-  </si>
-  <si>
-    <t>นายชาติเวท</t>
-  </si>
-  <si>
-    <t>สายบุตร</t>
-  </si>
-  <si>
-    <t>นางสาวเชฬุณีย์</t>
-  </si>
-  <si>
-    <t>ภูวฐิตานนท์</t>
-  </si>
-  <si>
-    <t>นางสาวฌัชชา</t>
-  </si>
-  <si>
-    <t>มาลารัตน์</t>
-  </si>
-  <si>
-    <t>นางสาวญาณิศา</t>
-  </si>
-  <si>
-    <t>ตาพรหม</t>
-  </si>
-  <si>
-    <t>นางสาวณัชชา</t>
-  </si>
-  <si>
-    <t>พาทพุทธิพงศ์</t>
-  </si>
-  <si>
-    <t>นางสาวณัฏฐธิดา</t>
-  </si>
-  <si>
-    <t>วณิชพิพัฒน์กุล</t>
-  </si>
-  <si>
-    <t>นางสาวณัฏฐนิช</t>
-  </si>
-  <si>
-    <t>บุญแร่</t>
-  </si>
-  <si>
-    <t>นายณัฐพงศ์</t>
-  </si>
-  <si>
-    <t>ปันยศ</t>
-  </si>
-  <si>
-    <t>นางสาวทิพย์ธิดา</t>
-  </si>
-  <si>
-    <t>แซ่เติ๋น</t>
-  </si>
-  <si>
-    <t>นายธุววิช</t>
-  </si>
-  <si>
-    <t>ปานเกิด</t>
-  </si>
-  <si>
-    <t>นางสาวนัยนา</t>
-  </si>
-  <si>
-    <t>สิทธิเจริญ</t>
-  </si>
-  <si>
-    <t>นางสาวนิธิพร</t>
-  </si>
-  <si>
-    <t>จันทะวัง</t>
-  </si>
-  <si>
-    <t>นายปรเมทฎ</t>
-  </si>
-  <si>
-    <t>นิติประศาสน์</t>
-  </si>
-  <si>
-    <t>นายปราชญ์</t>
-  </si>
-  <si>
-    <t>หลิ่มสุริยะ</t>
-  </si>
-  <si>
-    <t>นางสาวปริญญ์</t>
-  </si>
-  <si>
-    <t>รัตตัญญู</t>
-  </si>
-  <si>
-    <t>นางสาวปริยาภัทร</t>
-  </si>
-  <si>
-    <t>สมบัติปัน</t>
-  </si>
-  <si>
-    <t>นางสาวปวีณ์นุช</t>
-  </si>
-  <si>
-    <t>เอื้อแท้</t>
-  </si>
-  <si>
-    <t>นางสาวปวีณ์สุดา</t>
-  </si>
-  <si>
-    <t>เดชบุญ</t>
-  </si>
-  <si>
-    <t>นางสาวปิยธิดา</t>
-  </si>
-  <si>
-    <t>คำน้อย</t>
-  </si>
-  <si>
-    <t>นายปุริม</t>
-  </si>
-  <si>
-    <t>วาดเขียน</t>
-  </si>
-  <si>
-    <t>นายพงศกร</t>
-  </si>
-  <si>
-    <t>ยั่งยืน</t>
-  </si>
-  <si>
-    <t>นางสาวพัชราวลัย</t>
-  </si>
-  <si>
-    <t>เด่นนิติรัตน์</t>
-  </si>
-  <si>
-    <t>นางสาวพัชรี</t>
-  </si>
-  <si>
-    <t>อิสาน</t>
-  </si>
-  <si>
-    <t>นางสาวพิจาริน</t>
-  </si>
-  <si>
-    <t>ศิริพจนานนท์</t>
-  </si>
-  <si>
-    <t>นายพิชญ์ยุติ</t>
-  </si>
-  <si>
-    <t>ใจมิภักดิ์</t>
-  </si>
-  <si>
-    <t>นางสาวมัลลิกา</t>
-  </si>
-  <si>
-    <t>ไชยบัง</t>
-  </si>
-  <si>
-    <t>นายยศกร</t>
-  </si>
-  <si>
-    <t>สุดสวาสดิ์</t>
-  </si>
-  <si>
-    <t>นายเยาวยุทธ์</t>
-  </si>
-  <si>
-    <t>กันธัง</t>
-  </si>
-  <si>
-    <t>นางสาวรวินันท์</t>
-  </si>
-  <si>
-    <t>อุ้ยประเสริฐวัฒนา</t>
-  </si>
-  <si>
-    <t>นายฤทธิพร</t>
-  </si>
-  <si>
-    <t>จันทร์ขจร</t>
-  </si>
-  <si>
-    <t>นางสาวลภัสนันท์</t>
-  </si>
-  <si>
-    <t>พิราดา</t>
-  </si>
-  <si>
-    <t>นายสามารถ</t>
-  </si>
-  <si>
-    <t>สนิทมาก</t>
-  </si>
-  <si>
-    <t>นางสาวสิริกานดา</t>
-  </si>
-  <si>
-    <t>กล้าวิกย์การ</t>
-  </si>
-  <si>
-    <t>อุ่นจิต</t>
-  </si>
-  <si>
-    <t>นางสาวสุทธิพร</t>
-  </si>
-  <si>
-    <t>มณีวงค์</t>
-  </si>
-  <si>
-    <t>นายสุทธิศักดิ์</t>
-  </si>
-  <si>
-    <t>สิริกุลสัมพันธ์</t>
-  </si>
-  <si>
-    <t>นางสาวสุทธิษา</t>
-  </si>
-  <si>
-    <t>มณีรัตน์</t>
-  </si>
-  <si>
-    <t>นางสาวอัจฉราพรรณ</t>
-  </si>
-  <si>
-    <t>คำแก้ว</t>
-  </si>
-  <si>
-    <t>นางสาวเอกรณี</t>
-  </si>
-  <si>
-    <t>ขัดเรือง</t>
-  </si>
-  <si>
-    <t>นางสาวเอมวรี</t>
-  </si>
-  <si>
-    <t>มีชัยสุวรรณ์</t>
-  </si>
-  <si>
-    <t>นางสาวประกายกานต์</t>
-  </si>
-  <si>
-    <t>ศรีสองสกุล</t>
-  </si>
-  <si>
-    <t>นางสาวประกายดาว</t>
-  </si>
-  <si>
-    <t>มากาศ</t>
-  </si>
-  <si>
-    <t>นางสาวพราวพิไล</t>
-  </si>
-  <si>
-    <t>เดชธงไชย</t>
-  </si>
-  <si>
-    <t>นางสาวมนัชยา</t>
-  </si>
-  <si>
-    <t>ยะโกะ</t>
-  </si>
-  <si>
-    <t>นางสาวเมธาวี</t>
-  </si>
-  <si>
-    <t>แสงทอง</t>
+    <t>ราชา</t>
+  </si>
+  <si>
+    <t>นางสาวเกศริน</t>
+  </si>
+  <si>
+    <t>นินชัย</t>
+  </si>
+  <si>
+    <t>นางสาวแกมกมล</t>
+  </si>
+  <si>
+    <t>ไชยกันทา</t>
+  </si>
+  <si>
+    <t>นางสาวนลินนิภา</t>
+  </si>
+  <si>
+    <t>แก้วสุตัน</t>
+  </si>
+  <si>
+    <t>นางสาวนันท์นภัส</t>
+  </si>
+  <si>
+    <t>ตันพฤทธิอนันต์</t>
+  </si>
+  <si>
+    <t>นายเนติพงศ์</t>
+  </si>
+  <si>
+    <t>โปร่งใจ</t>
+  </si>
+  <si>
+    <t>นางสาวปฏิมาภรณ์</t>
+  </si>
+  <si>
+    <t>สุคำ</t>
+  </si>
+  <si>
+    <t>นางสาวปภัสสร</t>
+  </si>
+  <si>
+    <t>ลิมป์ภัสสร</t>
+  </si>
+  <si>
+    <t>นางสาวปวีณสุดา</t>
+  </si>
+  <si>
+    <t>ศักดี</t>
+  </si>
+  <si>
+    <t>นางสาวปัทมาสน์</t>
+  </si>
+  <si>
+    <t>แก้วกัน</t>
+  </si>
+  <si>
+    <t>นายปิยะวิชญ์</t>
+  </si>
+  <si>
+    <t>ทรงประกอบ</t>
+  </si>
+  <si>
+    <t>นางสาวผาณิต</t>
+  </si>
+  <si>
+    <t>อินต๊ะเส็น</t>
+  </si>
+  <si>
+    <t>นางสาวพษพร</t>
+  </si>
+  <si>
+    <t>พิงพราวลี</t>
+  </si>
+  <si>
+    <t>นางสาววลีรัตน์</t>
+  </si>
+  <si>
+    <t>ธรรมสุพิลม</t>
+  </si>
+  <si>
+    <t>นายเศรษฐพงษ์</t>
+  </si>
+  <si>
+    <t>อภิมงคลเลิศ</t>
+  </si>
+  <si>
+    <t>นางสาวธัญพิชชา</t>
+  </si>
+  <si>
+    <t>โชติพฤกษ์</t>
+  </si>
+  <si>
+    <t>นางสาวปภัสรินทร์</t>
+  </si>
+  <si>
+    <t>จิรธีระพันธ์</t>
+  </si>
+  <si>
+    <t>นางสาวปริยลักษณ์</t>
+  </si>
+  <si>
+    <t>จันทราภา</t>
+  </si>
+  <si>
+    <t>นางสาวปวิตรา</t>
+  </si>
+  <si>
+    <t>ลิมป์เติมทรัพย์</t>
+  </si>
+  <si>
+    <t>นางสาวปาณฑรา</t>
+  </si>
+  <si>
+    <t>กันสาย</t>
+  </si>
+  <si>
+    <t>นางสาวพรนิภา</t>
+  </si>
+  <si>
+    <t>ขุนนาพุ่ม</t>
+  </si>
+  <si>
+    <t>นางสาวมณฑกาญจน์</t>
+  </si>
+  <si>
+    <t>ปัญญาฟู</t>
+  </si>
+  <si>
+    <t>นายไม้น้ำ</t>
+  </si>
+  <si>
+    <t>สุวรรณจุณีย์</t>
+  </si>
+  <si>
+    <t>นางสาวรจิตา</t>
+  </si>
+  <si>
+    <t>ป๊อกคำอู๋</t>
+  </si>
+  <si>
+    <t>นางสาวรัชดาพร</t>
+  </si>
+  <si>
+    <t>เพ็ญสว่าง</t>
+  </si>
+  <si>
+    <t>นางสาววชิรญาณ์</t>
+  </si>
+  <si>
+    <t>บำเพ็ญอยู่</t>
+  </si>
+  <si>
+    <t>นายวรเมธ</t>
+  </si>
+  <si>
+    <t>สกุลงาม</t>
+  </si>
+  <si>
+    <t>นางสาววารุณี</t>
+  </si>
+  <si>
+    <t>สมนวล</t>
+  </si>
+  <si>
+    <t>นางสาวศศิวิมล</t>
+  </si>
+  <si>
+    <t>พรมพฤกษ์</t>
+  </si>
+  <si>
+    <t>นายศิรวุฒิ</t>
+  </si>
+  <si>
+    <t>จิตต์ใจ</t>
+  </si>
+  <si>
+    <t>นายศุภชัย</t>
+  </si>
+  <si>
+    <t>เปรมศรี</t>
+  </si>
+  <si>
+    <t>นางสาวศุภิสรา</t>
+  </si>
+  <si>
+    <t>นิลขำ</t>
+  </si>
+  <si>
+    <t>นางสาวสกุลรัตน์</t>
+  </si>
+  <si>
+    <t>หัดเคลือบ</t>
+  </si>
+  <si>
+    <t>นายสรศักดิ์</t>
+  </si>
+  <si>
+    <t>อินต๊ะแก้ว</t>
+  </si>
+  <si>
+    <t>นางสาวสิริกุล</t>
+  </si>
+  <si>
+    <t>พรหมกันธา</t>
+  </si>
+  <si>
+    <t>นางสาวสุทฐิญาภรณ์</t>
+  </si>
+  <si>
+    <t>กิตติกรวัฒนา</t>
+  </si>
+  <si>
+    <t>นางสาวสุธาทิพย์</t>
+  </si>
+  <si>
+    <t>ศรีธรรมมา</t>
+  </si>
+  <si>
+    <t>นายสุธิพันธ์</t>
+  </si>
+  <si>
+    <t>แก้วจันทร์เพชร</t>
+  </si>
+  <si>
+    <t>นายอนุรักษ์</t>
+  </si>
+  <si>
+    <t>รังษี</t>
+  </si>
+  <si>
+    <t>นางสาวอภิชญา</t>
+  </si>
+  <si>
+    <t>ปันจันทร์</t>
+  </si>
+  <si>
+    <t>นายอภิรักษ์</t>
+  </si>
+  <si>
+    <t>วงศ์พันธุ์</t>
+  </si>
+  <si>
+    <t>นายอภิสิทธิ์</t>
+  </si>
+  <si>
+    <t>พวงมาลัย</t>
+  </si>
+  <si>
+    <t>นางสาวอรพรรณ</t>
+  </si>
+  <si>
+    <t>พงษ์กิจการุณ</t>
+  </si>
+  <si>
+    <t>นางสาวอลิศา</t>
+  </si>
+  <si>
+    <t>ศรีระวัตร</t>
+  </si>
+  <si>
+    <t>นางสาวอัจฉรี</t>
+  </si>
+  <si>
+    <t>บัวเขียว</t>
+  </si>
+  <si>
+    <t>นายอานุภาพ</t>
+  </si>
+  <si>
+    <t>พลวัน</t>
+  </si>
+  <si>
+    <t>นายอุกฤษณ์</t>
+  </si>
+  <si>
+    <t>วัชรวิเชษฐ์</t>
+  </si>
+  <si>
+    <t>นายณัฐภัทร</t>
+  </si>
+  <si>
+    <t>นะที</t>
+  </si>
+  <si>
+    <t>นายเพิ่มธนา</t>
+  </si>
+  <si>
+    <t>สดใส</t>
   </si>
 </sst>
 </file>
@@ -1085,10 +1340,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F98"/>
+  <dimension ref="A1:F142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="F98" sqref="F98"/>
+      <selection activeCell="F142" sqref="F142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1181,7 +1436,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="11">
-        <v>531910135</v>
+        <v>540110214</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>14</v>
@@ -1198,7 +1453,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="11">
-        <v>540510297</v>
+        <v>540110217</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>17</v>
@@ -1207,7 +1462,7 @@
         <v>18</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:6" customHeight="1" ht="19.8">
@@ -1215,16 +1470,16 @@
         <v>3</v>
       </c>
       <c r="C10" s="11">
-        <v>540510305</v>
+        <v>540110222</v>
       </c>
       <c r="D10" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="13" t="s">
-        <v>21</v>
-      </c>
       <c r="F10" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:6" customHeight="1" ht="19.8">
@@ -1232,16 +1487,16 @@
         <v>4</v>
       </c>
       <c r="C11" s="11">
-        <v>540510669</v>
+        <v>540110224</v>
       </c>
       <c r="D11" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="13" t="s">
-        <v>23</v>
-      </c>
       <c r="F11" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:6" customHeight="1" ht="19.8">
@@ -1249,16 +1504,16 @@
         <v>5</v>
       </c>
       <c r="C12" s="11">
-        <v>550210003</v>
+        <v>550310177</v>
       </c>
       <c r="D12" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="F12" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:6" customHeight="1" ht="19.8">
@@ -1266,16 +1521,16 @@
         <v>6</v>
       </c>
       <c r="C13" s="11">
-        <v>550210012</v>
+        <v>550310183</v>
       </c>
       <c r="D13" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="13" t="s">
-        <v>27</v>
-      </c>
       <c r="F13" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:6" customHeight="1" ht="19.8">
@@ -1283,16 +1538,16 @@
         <v>7</v>
       </c>
       <c r="C14" s="11">
-        <v>551310113</v>
+        <v>550310192</v>
       </c>
       <c r="D14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="13" t="s">
-        <v>29</v>
-      </c>
       <c r="F14" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:6" customHeight="1" ht="19.8">
@@ -1300,16 +1555,16 @@
         <v>8</v>
       </c>
       <c r="C15" s="11">
-        <v>560510019</v>
+        <v>550310223</v>
       </c>
       <c r="D15" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="13" t="s">
-        <v>31</v>
-      </c>
       <c r="F15" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:6" customHeight="1" ht="19.8">
@@ -1317,16 +1572,16 @@
         <v>9</v>
       </c>
       <c r="C16" s="11">
-        <v>560510615</v>
+        <v>551611058</v>
       </c>
       <c r="D16" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="13" t="s">
-        <v>33</v>
-      </c>
       <c r="F16" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:6" customHeight="1" ht="19.8">
@@ -1334,16 +1589,16 @@
         <v>10</v>
       </c>
       <c r="C17" s="11">
-        <v>561010050</v>
+        <v>551611060</v>
       </c>
       <c r="D17" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="13" t="s">
-        <v>35</v>
-      </c>
       <c r="F17" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:6" customHeight="1" ht="19.8">
@@ -1351,16 +1606,16 @@
         <v>11</v>
       </c>
       <c r="C18" s="11">
-        <v>561010160</v>
+        <v>551611063</v>
       </c>
       <c r="D18" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="13" t="s">
-        <v>37</v>
-      </c>
       <c r="F18" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:6" customHeight="1" ht="19.8">
@@ -1368,16 +1623,16 @@
         <v>12</v>
       </c>
       <c r="C19" s="11">
-        <v>561611090</v>
+        <v>560110112</v>
       </c>
       <c r="D19" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="13" t="s">
-        <v>39</v>
-      </c>
       <c r="F19" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:6" customHeight="1" ht="19.8">
@@ -1385,16 +1640,16 @@
         <v>13</v>
       </c>
       <c r="C20" s="11">
-        <v>570110135</v>
+        <v>560110119</v>
       </c>
       <c r="D20" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="13" t="s">
-        <v>41</v>
-      </c>
       <c r="F20" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:6" customHeight="1" ht="19.8">
@@ -1402,16 +1657,16 @@
         <v>14</v>
       </c>
       <c r="C21" s="11">
-        <v>570110144</v>
+        <v>560410001</v>
       </c>
       <c r="D21" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="13" t="s">
-        <v>43</v>
-      </c>
       <c r="F21" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:6" customHeight="1" ht="19.8">
@@ -1419,16 +1674,16 @@
         <v>15</v>
       </c>
       <c r="C22" s="11">
-        <v>570110156</v>
+        <v>560410012</v>
       </c>
       <c r="D22" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="13" t="s">
-        <v>45</v>
-      </c>
       <c r="F22" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:6" customHeight="1" ht="19.8">
@@ -1436,16 +1691,16 @@
         <v>16</v>
       </c>
       <c r="C23" s="11">
-        <v>570110213</v>
+        <v>560410014</v>
       </c>
       <c r="D23" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="13" t="s">
-        <v>47</v>
-      </c>
       <c r="F23" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:6" customHeight="1" ht="19.8">
@@ -1453,16 +1708,16 @@
         <v>17</v>
       </c>
       <c r="C24" s="11">
-        <v>570210060</v>
+        <v>560410030</v>
       </c>
       <c r="D24" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E24" s="13" t="s">
-        <v>49</v>
-      </c>
       <c r="F24" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:6" customHeight="1" ht="19.8">
@@ -1470,16 +1725,16 @@
         <v>18</v>
       </c>
       <c r="C25" s="11">
-        <v>570510620</v>
+        <v>560410034</v>
       </c>
       <c r="D25" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E25" s="13" t="s">
-        <v>51</v>
-      </c>
       <c r="F25" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:6" customHeight="1" ht="19.8">
@@ -1487,16 +1742,16 @@
         <v>19</v>
       </c>
       <c r="C26" s="11">
-        <v>570510629</v>
+        <v>560410039</v>
       </c>
       <c r="D26" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E26" s="13" t="s">
-        <v>53</v>
-      </c>
       <c r="F26" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:6" customHeight="1" ht="19.8">
@@ -1504,16 +1759,16 @@
         <v>20</v>
       </c>
       <c r="C27" s="11">
-        <v>570510635</v>
+        <v>560410044</v>
       </c>
       <c r="D27" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="13" t="s">
-        <v>55</v>
-      </c>
       <c r="F27" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:6" customHeight="1" ht="19.8">
@@ -1521,16 +1776,16 @@
         <v>21</v>
       </c>
       <c r="C28" s="11">
-        <v>570510640</v>
+        <v>560410049</v>
       </c>
       <c r="D28" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="E28" s="13" t="s">
-        <v>57</v>
-      </c>
       <c r="F28" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:6" customHeight="1" ht="19.8">
@@ -1538,16 +1793,16 @@
         <v>22</v>
       </c>
       <c r="C29" s="11">
-        <v>570510643</v>
+        <v>560410052</v>
       </c>
       <c r="D29" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E29" s="13" t="s">
-        <v>59</v>
-      </c>
       <c r="F29" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:6" customHeight="1" ht="19.8">
@@ -1555,16 +1810,16 @@
         <v>23</v>
       </c>
       <c r="C30" s="11">
-        <v>570510680</v>
+        <v>560410053</v>
       </c>
       <c r="D30" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E30" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E30" s="13" t="s">
-        <v>61</v>
-      </c>
       <c r="F30" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:6" customHeight="1" ht="19.8">
@@ -1572,16 +1827,16 @@
         <v>24</v>
       </c>
       <c r="C31" s="11">
-        <v>570510694</v>
+        <v>560410057</v>
       </c>
       <c r="D31" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="13" t="s">
-        <v>63</v>
-      </c>
       <c r="F31" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:6" customHeight="1" ht="19.8">
@@ -1589,16 +1844,16 @@
         <v>25</v>
       </c>
       <c r="C32" s="11">
-        <v>571110013</v>
+        <v>560410061</v>
       </c>
       <c r="D32" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="E32" s="13" t="s">
-        <v>65</v>
-      </c>
       <c r="F32" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:6" customHeight="1" ht="19.8">
@@ -1606,16 +1861,16 @@
         <v>26</v>
       </c>
       <c r="C33" s="11">
-        <v>571110019</v>
+        <v>560410064</v>
       </c>
       <c r="D33" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="E33" s="13" t="s">
-        <v>67</v>
-      </c>
       <c r="F33" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:6" customHeight="1" ht="19.8">
@@ -1623,16 +1878,16 @@
         <v>27</v>
       </c>
       <c r="C34" s="11">
-        <v>571110039</v>
+        <v>560410090</v>
       </c>
       <c r="D34" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E34" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="E34" s="13" t="s">
-        <v>69</v>
-      </c>
       <c r="F34" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:6" customHeight="1" ht="19.8">
@@ -1640,16 +1895,16 @@
         <v>28</v>
       </c>
       <c r="C35" s="11">
-        <v>571110097</v>
+        <v>560410091</v>
       </c>
       <c r="D35" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E35" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="E35" s="13" t="s">
-        <v>71</v>
-      </c>
       <c r="F35" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:6" customHeight="1" ht="19.8">
@@ -1657,16 +1912,16 @@
         <v>29</v>
       </c>
       <c r="C36" s="11">
-        <v>571110101</v>
+        <v>560410112</v>
       </c>
       <c r="D36" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="E36" s="13" t="s">
-        <v>73</v>
-      </c>
       <c r="F36" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1687,16 +1942,16 @@
         <v>30</v>
       </c>
       <c r="C38" s="11">
-        <v>571110102</v>
+        <v>560410118</v>
       </c>
       <c r="D38" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="E38" s="13" t="s">
-        <v>75</v>
-      </c>
       <c r="F38" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:6" customHeight="1" ht="19.8">
@@ -1704,16 +1959,16 @@
         <v>31</v>
       </c>
       <c r="C39" s="11">
-        <v>571110103</v>
+        <v>560410132</v>
       </c>
       <c r="D39" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E39" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E39" s="13" t="s">
-        <v>77</v>
-      </c>
       <c r="F39" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:6" customHeight="1" ht="19.8">
@@ -1721,16 +1976,16 @@
         <v>32</v>
       </c>
       <c r="C40" s="11">
-        <v>571110104</v>
+        <v>561910066</v>
       </c>
       <c r="D40" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="E40" s="13" t="s">
-        <v>79</v>
-      </c>
       <c r="F40" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:6" customHeight="1" ht="19.8">
@@ -1738,16 +1993,16 @@
         <v>33</v>
       </c>
       <c r="C41" s="11">
-        <v>571110105</v>
+        <v>561910069</v>
       </c>
       <c r="D41" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E41" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="E41" s="13" t="s">
-        <v>81</v>
-      </c>
       <c r="F41" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:6" customHeight="1" ht="19.8">
@@ -1755,16 +2010,16 @@
         <v>34</v>
       </c>
       <c r="C42" s="11">
-        <v>571110108</v>
+        <v>561910081</v>
       </c>
       <c r="D42" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E42" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="E42" s="13" t="s">
-        <v>83</v>
-      </c>
       <c r="F42" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:6" customHeight="1" ht="19.8">
@@ -1772,16 +2027,16 @@
         <v>35</v>
       </c>
       <c r="C43" s="11">
-        <v>571110109</v>
+        <v>561910102</v>
       </c>
       <c r="D43" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E43" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="E43" s="13" t="s">
-        <v>85</v>
-      </c>
       <c r="F43" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:6" customHeight="1" ht="19.8">
@@ -1789,16 +2044,16 @@
         <v>36</v>
       </c>
       <c r="C44" s="11">
-        <v>571510251</v>
+        <v>561910119</v>
       </c>
       <c r="D44" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E44" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="E44" s="13" t="s">
-        <v>87</v>
-      </c>
       <c r="F44" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:6" customHeight="1" ht="19.8">
@@ -1806,16 +2061,16 @@
         <v>37</v>
       </c>
       <c r="C45" s="11">
-        <v>571510259</v>
+        <v>561910121</v>
       </c>
       <c r="D45" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E45" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="E45" s="13" t="s">
-        <v>89</v>
-      </c>
       <c r="F45" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:6" customHeight="1" ht="19.8">
@@ -1823,16 +2078,16 @@
         <v>38</v>
       </c>
       <c r="C46" s="11">
-        <v>571510260</v>
+        <v>570110245</v>
       </c>
       <c r="D46" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E46" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="E46" s="13" t="s">
-        <v>91</v>
-      </c>
       <c r="F46" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:6" customHeight="1" ht="19.8">
@@ -1840,16 +2095,16 @@
         <v>39</v>
       </c>
       <c r="C47" s="11">
-        <v>571810015</v>
+        <v>570110246</v>
       </c>
       <c r="D47" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="E47" s="13" t="s">
-        <v>93</v>
-      </c>
       <c r="F47" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:6" customHeight="1" ht="19.8">
@@ -1857,16 +2112,16 @@
         <v>40</v>
       </c>
       <c r="C48" s="11">
-        <v>571810017</v>
+        <v>570110247</v>
       </c>
       <c r="D48" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E48" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="E48" s="13" t="s">
-        <v>95</v>
-      </c>
       <c r="F48" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:6" customHeight="1" ht="19.8">
@@ -1874,16 +2129,16 @@
         <v>41</v>
       </c>
       <c r="C49" s="11">
-        <v>571810019</v>
+        <v>570110248</v>
       </c>
       <c r="D49" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E49" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="E49" s="13" t="s">
-        <v>97</v>
-      </c>
       <c r="F49" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:6" customHeight="1" ht="19.8">
@@ -1891,16 +2146,16 @@
         <v>42</v>
       </c>
       <c r="C50" s="11">
-        <v>571810030</v>
+        <v>570110250</v>
       </c>
       <c r="D50" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E50" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="E50" s="13" t="s">
-        <v>99</v>
-      </c>
       <c r="F50" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:6" customHeight="1" ht="19.8">
@@ -1908,16 +2163,16 @@
         <v>43</v>
       </c>
       <c r="C51" s="11">
-        <v>571810031</v>
+        <v>570110251</v>
       </c>
       <c r="D51" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E51" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="E51" s="13" t="s">
-        <v>101</v>
-      </c>
       <c r="F51" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:6" customHeight="1" ht="19.8">
@@ -1925,16 +2180,16 @@
         <v>44</v>
       </c>
       <c r="C52" s="11">
-        <v>571810036</v>
+        <v>570110252</v>
       </c>
       <c r="D52" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="E52" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="E52" s="13" t="s">
-        <v>103</v>
-      </c>
       <c r="F52" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:6" customHeight="1" ht="19.8">
@@ -1942,16 +2197,16 @@
         <v>45</v>
       </c>
       <c r="C53" s="11">
-        <v>571810038</v>
+        <v>570110253</v>
       </c>
       <c r="D53" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E53" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="E53" s="13" t="s">
-        <v>105</v>
-      </c>
       <c r="F53" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:6" customHeight="1" ht="19.8">
@@ -1959,16 +2214,16 @@
         <v>46</v>
       </c>
       <c r="C54" s="11">
-        <v>571810042</v>
+        <v>570110402</v>
       </c>
       <c r="D54" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="E54" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="E54" s="13" t="s">
-        <v>107</v>
-      </c>
       <c r="F54" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:6" customHeight="1" ht="19.8">
@@ -1976,16 +2231,16 @@
         <v>47</v>
       </c>
       <c r="C55" s="11">
-        <v>571810043</v>
+        <v>570110418</v>
       </c>
       <c r="D55" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E55" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="E55" s="13" t="s">
-        <v>109</v>
-      </c>
       <c r="F55" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:6" customHeight="1" ht="19.8">
@@ -1993,16 +2248,16 @@
         <v>48</v>
       </c>
       <c r="C56" s="11">
-        <v>571810045</v>
+        <v>570210134</v>
       </c>
       <c r="D56" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E56" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="E56" s="13" t="s">
-        <v>111</v>
-      </c>
       <c r="F56" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:6" customHeight="1" ht="19.8">
@@ -2010,16 +2265,16 @@
         <v>49</v>
       </c>
       <c r="C57" s="11">
-        <v>571810053</v>
+        <v>570810005</v>
       </c>
       <c r="D57" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E57" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="E57" s="13" t="s">
-        <v>113</v>
-      </c>
       <c r="F57" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:6" customHeight="1" ht="19.8">
@@ -2027,16 +2282,16 @@
         <v>50</v>
       </c>
       <c r="C58" s="11">
-        <v>571810056</v>
+        <v>570810024</v>
       </c>
       <c r="D58" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E58" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="E58" s="13" t="s">
-        <v>115</v>
-      </c>
       <c r="F58" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59" spans="1:6" customHeight="1" ht="19.8">
@@ -2044,16 +2299,16 @@
         <v>51</v>
       </c>
       <c r="C59" s="11">
-        <v>571810057</v>
+        <v>570810049</v>
       </c>
       <c r="D59" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="E59" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="E59" s="13" t="s">
-        <v>117</v>
-      </c>
       <c r="F59" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="60" spans="1:6" customHeight="1" ht="19.8">
@@ -2061,16 +2316,16 @@
         <v>52</v>
       </c>
       <c r="C60" s="11">
-        <v>571810062</v>
+        <v>570810052</v>
       </c>
       <c r="D60" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E60" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E60" s="13" t="s">
-        <v>119</v>
-      </c>
       <c r="F60" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:6" customHeight="1" ht="19.8">
@@ -2078,16 +2333,16 @@
         <v>53</v>
       </c>
       <c r="C61" s="11">
-        <v>571810069</v>
+        <v>570810062</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>120</v>
+        <v>63</v>
       </c>
       <c r="E61" s="13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F61" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:6" customHeight="1" ht="19.8">
@@ -2095,16 +2350,16 @@
         <v>54</v>
       </c>
       <c r="C62" s="11">
-        <v>571810085</v>
+        <v>570810064</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E62" s="13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F62" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="63" spans="1:6" customHeight="1" ht="19.8">
@@ -2112,16 +2367,16 @@
         <v>55</v>
       </c>
       <c r="C63" s="11">
-        <v>571810093</v>
+        <v>570810067</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E63" s="13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F63" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:6" customHeight="1" ht="19.8">
@@ -2129,16 +2384,16 @@
         <v>56</v>
       </c>
       <c r="C64" s="11">
-        <v>571810094</v>
+        <v>570810080</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E64" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F64" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:6" customHeight="1" ht="19.8">
@@ -2146,16 +2401,16 @@
         <v>57</v>
       </c>
       <c r="C65" s="11">
-        <v>571810104</v>
+        <v>570810083</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E65" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F65" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="66" spans="1:6" customHeight="1" ht="19.8">
@@ -2163,16 +2418,16 @@
         <v>58</v>
       </c>
       <c r="C66" s="11">
-        <v>571810105</v>
+        <v>570810090</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E66" s="13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="67" spans="1:6" customHeight="1" ht="19.8">
@@ -2180,16 +2435,16 @@
         <v>59</v>
       </c>
       <c r="C67" s="11">
-        <v>571810106</v>
+        <v>570810101</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E67" s="13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F67" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="68" spans="1:6" customHeight="1" ht="19.8">
@@ -2197,16 +2452,16 @@
         <v>60</v>
       </c>
       <c r="C68" s="11">
-        <v>571810107</v>
+        <v>570810172</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E68" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F68" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="69" spans="1:6" customHeight="1" ht="19.8">
@@ -2214,16 +2469,16 @@
         <v>61</v>
       </c>
       <c r="C69" s="11">
-        <v>571810110</v>
+        <v>570810209</v>
       </c>
       <c r="D69" s="12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E69" s="13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F69" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="70" spans="1:6" customHeight="1" ht="19.8">
@@ -2231,16 +2486,16 @@
         <v>62</v>
       </c>
       <c r="C70" s="11">
-        <v>571810111</v>
+        <v>570810210</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E70" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F70" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:6" customHeight="1" ht="19.8">
@@ -2248,16 +2503,16 @@
         <v>63</v>
       </c>
       <c r="C71" s="11">
-        <v>571810113</v>
+        <v>570810351</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E71" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F71" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:6" customHeight="1" ht="19.8">
@@ -2265,16 +2520,16 @@
         <v>64</v>
       </c>
       <c r="C72" s="11">
-        <v>571810114</v>
+        <v>570810352</v>
       </c>
       <c r="D72" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E72" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F72" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2295,16 +2550,16 @@
         <v>65</v>
       </c>
       <c r="C74" s="11">
-        <v>571810115</v>
+        <v>570810360</v>
       </c>
       <c r="D74" s="12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E74" s="13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:6" customHeight="1" ht="19.8">
@@ -2312,16 +2567,16 @@
         <v>66</v>
       </c>
       <c r="C75" s="11">
-        <v>571810120</v>
+        <v>570810361</v>
       </c>
       <c r="D75" s="12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E75" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F75" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="76" spans="1:6" customHeight="1" ht="19.8">
@@ -2329,16 +2584,16 @@
         <v>67</v>
       </c>
       <c r="C76" s="11">
-        <v>571810121</v>
+        <v>570810362</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E76" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F76" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="77" spans="1:6" customHeight="1" ht="19.8">
@@ -2346,16 +2601,16 @@
         <v>68</v>
       </c>
       <c r="C77" s="11">
-        <v>571810122</v>
+        <v>570810366</v>
       </c>
       <c r="D77" s="12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E77" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F77" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="78" spans="1:6" customHeight="1" ht="19.8">
@@ -2363,13 +2618,13 @@
         <v>69</v>
       </c>
       <c r="C78" s="11">
-        <v>571810124</v>
+        <v>570810368</v>
       </c>
       <c r="D78" s="12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E78" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F78" s="11" t="s">
         <v>16</v>
@@ -2380,16 +2635,16 @@
         <v>70</v>
       </c>
       <c r="C79" s="11">
-        <v>571810141</v>
+        <v>571410002</v>
       </c>
       <c r="D79" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E79" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F79" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="80" spans="1:6" customHeight="1" ht="19.8">
@@ -2397,16 +2652,16 @@
         <v>71</v>
       </c>
       <c r="C80" s="11">
-        <v>571810143</v>
+        <v>571410013</v>
       </c>
       <c r="D80" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E80" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F80" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="81" spans="1:6" customHeight="1" ht="19.8">
@@ -2414,16 +2669,16 @@
         <v>72</v>
       </c>
       <c r="C81" s="11">
-        <v>571810144</v>
+        <v>571410015</v>
       </c>
       <c r="D81" s="12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E81" s="13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F81" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="82" spans="1:6" customHeight="1" ht="19.8">
@@ -2431,16 +2686,16 @@
         <v>73</v>
       </c>
       <c r="C82" s="11">
-        <v>571810148</v>
+        <v>571410033</v>
       </c>
       <c r="D82" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E82" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F82" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="83" spans="1:6" customHeight="1" ht="19.8">
@@ -2448,16 +2703,16 @@
         <v>74</v>
       </c>
       <c r="C83" s="11">
-        <v>571810155</v>
+        <v>571410037</v>
       </c>
       <c r="D83" s="12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E83" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F83" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="84" spans="1:6" customHeight="1" ht="19.8">
@@ -2465,16 +2720,16 @@
         <v>75</v>
       </c>
       <c r="C84" s="11">
-        <v>571810156</v>
+        <v>571410038</v>
       </c>
       <c r="D84" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E84" s="13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F84" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="85" spans="1:6" customHeight="1" ht="19.8">
@@ -2482,16 +2737,16 @@
         <v>76</v>
       </c>
       <c r="C85" s="11">
-        <v>571810181</v>
+        <v>571410051</v>
       </c>
       <c r="D85" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E85" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F85" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="86" spans="1:6" customHeight="1" ht="19.8">
@@ -2499,16 +2754,16 @@
         <v>77</v>
       </c>
       <c r="C86" s="11">
-        <v>571810182</v>
+        <v>571410052</v>
       </c>
       <c r="D86" s="12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E86" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F86" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="87" spans="1:6" customHeight="1" ht="19.8">
@@ -2516,16 +2771,16 @@
         <v>78</v>
       </c>
       <c r="C87" s="11">
-        <v>571810183</v>
+        <v>571410055</v>
       </c>
       <c r="D87" s="12" t="s">
-        <v>28</v>
+        <v>168</v>
       </c>
       <c r="E87" s="13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F87" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="88" spans="1:6" customHeight="1" ht="19.8">
@@ -2533,16 +2788,16 @@
         <v>79</v>
       </c>
       <c r="C88" s="11">
-        <v>571810184</v>
+        <v>571410057</v>
       </c>
       <c r="D88" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="E88" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="E88" s="13" t="s">
-        <v>172</v>
-      </c>
       <c r="F88" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="89" spans="1:6" customHeight="1" ht="19.8">
@@ -2550,16 +2805,16 @@
         <v>80</v>
       </c>
       <c r="C89" s="11">
-        <v>571810185</v>
+        <v>571610008</v>
       </c>
       <c r="D89" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="E89" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="E89" s="13" t="s">
-        <v>174</v>
-      </c>
       <c r="F89" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="90" spans="1:6" customHeight="1" ht="19.8">
@@ -2567,16 +2822,16 @@
         <v>81</v>
       </c>
       <c r="C90" s="11">
-        <v>571810186</v>
+        <v>571610013</v>
       </c>
       <c r="D90" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="E90" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="E90" s="13" t="s">
-        <v>176</v>
-      </c>
       <c r="F90" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="91" spans="1:6" customHeight="1" ht="19.8">
@@ -2584,16 +2839,16 @@
         <v>82</v>
       </c>
       <c r="C91" s="11">
-        <v>571810198</v>
+        <v>571610020</v>
       </c>
       <c r="D91" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="E91" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="E91" s="13" t="s">
-        <v>178</v>
-      </c>
       <c r="F91" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="92" spans="1:6" customHeight="1" ht="19.8">
@@ -2601,16 +2856,16 @@
         <v>83</v>
       </c>
       <c r="C92" s="11">
-        <v>571810204</v>
+        <v>571610021</v>
       </c>
       <c r="D92" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="E92" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="E92" s="13" t="s">
-        <v>180</v>
-      </c>
       <c r="F92" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="93" spans="1:6" customHeight="1" ht="19.8">
@@ -2618,16 +2873,16 @@
         <v>84</v>
       </c>
       <c r="C93" s="11">
-        <v>571810206</v>
+        <v>571610022</v>
       </c>
       <c r="D93" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="E93" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="E93" s="13" t="s">
-        <v>182</v>
-      </c>
       <c r="F93" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="94" spans="1:6" customHeight="1" ht="19.8">
@@ -2635,16 +2890,16 @@
         <v>85</v>
       </c>
       <c r="C94" s="11">
-        <v>571910222</v>
+        <v>571610024</v>
       </c>
       <c r="D94" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="E94" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="E94" s="13" t="s">
-        <v>184</v>
-      </c>
       <c r="F94" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="95" spans="1:6" customHeight="1" ht="19.8">
@@ -2652,16 +2907,16 @@
         <v>86</v>
       </c>
       <c r="C95" s="11">
-        <v>571910223</v>
+        <v>571610025</v>
       </c>
       <c r="D95" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="E95" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="E95" s="13" t="s">
-        <v>186</v>
-      </c>
       <c r="F95" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="96" spans="1:6" customHeight="1" ht="19.8">
@@ -2669,16 +2924,16 @@
         <v>87</v>
       </c>
       <c r="C96" s="11">
-        <v>571910233</v>
+        <v>571610152</v>
       </c>
       <c r="D96" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="E96" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="E96" s="13" t="s">
-        <v>188</v>
-      </c>
       <c r="F96" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="97" spans="1:6" customHeight="1" ht="19.8">
@@ -2686,16 +2941,16 @@
         <v>88</v>
       </c>
       <c r="C97" s="11">
-        <v>571910246</v>
+        <v>571610154</v>
       </c>
       <c r="D97" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="E97" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="E97" s="13" t="s">
-        <v>190</v>
-      </c>
       <c r="F97" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="98" spans="1:6" customHeight="1" ht="19.8">
@@ -2703,16 +2958,760 @@
         <v>89</v>
       </c>
       <c r="C98" s="11">
-        <v>571910248</v>
+        <v>571610162</v>
       </c>
       <c r="D98" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="E98" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="E98" s="13" t="s">
+      <c r="F98" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B99" s="10">
+        <v>90</v>
+      </c>
+      <c r="C99" s="11">
+        <v>571610170</v>
+      </c>
+      <c r="D99" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="F98" s="11" t="s">
-        <v>19</v>
+      <c r="E99" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="F99" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B100" s="10">
+        <v>91</v>
+      </c>
+      <c r="C100" s="11">
+        <v>571610175</v>
+      </c>
+      <c r="D100" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="E100" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="F100" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B101" s="10">
+        <v>92</v>
+      </c>
+      <c r="C101" s="11">
+        <v>571610187</v>
+      </c>
+      <c r="D101" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="E101" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="F101" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B102" s="10">
+        <v>93</v>
+      </c>
+      <c r="C102" s="11">
+        <v>571610190</v>
+      </c>
+      <c r="D102" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="E102" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="F102" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B103" s="10">
+        <v>94</v>
+      </c>
+      <c r="C103" s="11">
+        <v>571610198</v>
+      </c>
+      <c r="D103" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="E103" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="F103" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B104" s="10">
+        <v>95</v>
+      </c>
+      <c r="C104" s="11">
+        <v>571610200</v>
+      </c>
+      <c r="D104" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="E104" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="F104" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B105" s="10">
+        <v>96</v>
+      </c>
+      <c r="C105" s="11">
+        <v>571610212</v>
+      </c>
+      <c r="D105" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="E105" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="F105" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B106" s="10">
+        <v>97</v>
+      </c>
+      <c r="C106" s="11">
+        <v>571610290</v>
+      </c>
+      <c r="D106" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="E106" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="F106" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B107" s="10">
+        <v>98</v>
+      </c>
+      <c r="C107" s="11">
+        <v>571610326</v>
+      </c>
+      <c r="D107" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="E107" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="F107" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B108" s="10">
+        <v>99</v>
+      </c>
+      <c r="C108" s="11">
+        <v>571910213</v>
+      </c>
+      <c r="D108" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="E108" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="F108" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="B109" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E109" s="5"/>
+      <c r="F109" s="5"/>
+    </row>
+    <row r="110" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B110" s="10">
+        <v>100</v>
+      </c>
+      <c r="C110" s="11">
+        <v>571910220</v>
+      </c>
+      <c r="D110" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="E110" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="F110" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B111" s="10">
+        <v>101</v>
+      </c>
+      <c r="C111" s="11">
+        <v>571910224</v>
+      </c>
+      <c r="D111" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="E111" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="F111" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B112" s="10">
+        <v>102</v>
+      </c>
+      <c r="C112" s="11">
+        <v>571910226</v>
+      </c>
+      <c r="D112" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="E112" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="F112" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B113" s="10">
+        <v>103</v>
+      </c>
+      <c r="C113" s="11">
+        <v>571910228</v>
+      </c>
+      <c r="D113" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="E113" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="F113" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B114" s="10">
+        <v>104</v>
+      </c>
+      <c r="C114" s="11">
+        <v>571910232</v>
+      </c>
+      <c r="D114" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="E114" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="F114" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B115" s="10">
+        <v>105</v>
+      </c>
+      <c r="C115" s="11">
+        <v>571910244</v>
+      </c>
+      <c r="D115" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="E115" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="F115" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B116" s="10">
+        <v>106</v>
+      </c>
+      <c r="C116" s="11">
+        <v>571910249</v>
+      </c>
+      <c r="D116" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="E116" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="F116" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B117" s="10">
+        <v>107</v>
+      </c>
+      <c r="C117" s="11">
+        <v>571910250</v>
+      </c>
+      <c r="D117" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="E117" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="F117" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B118" s="10">
+        <v>108</v>
+      </c>
+      <c r="C118" s="11">
+        <v>571910252</v>
+      </c>
+      <c r="D118" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="E118" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="F118" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B119" s="10">
+        <v>109</v>
+      </c>
+      <c r="C119" s="11">
+        <v>571910254</v>
+      </c>
+      <c r="D119" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="E119" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="F119" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B120" s="10">
+        <v>110</v>
+      </c>
+      <c r="C120" s="11">
+        <v>571910257</v>
+      </c>
+      <c r="D120" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="E120" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="F120" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B121" s="10">
+        <v>111</v>
+      </c>
+      <c r="C121" s="11">
+        <v>571910263</v>
+      </c>
+      <c r="D121" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="E121" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="F121" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B122" s="10">
+        <v>112</v>
+      </c>
+      <c r="C122" s="11">
+        <v>571910267</v>
+      </c>
+      <c r="D122" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="E122" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="F122" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B123" s="10">
+        <v>113</v>
+      </c>
+      <c r="C123" s="11">
+        <v>571910268</v>
+      </c>
+      <c r="D123" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="E123" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="F123" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B124" s="10">
+        <v>114</v>
+      </c>
+      <c r="C124" s="11">
+        <v>571910269</v>
+      </c>
+      <c r="D124" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="E124" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="F124" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B125" s="10">
+        <v>115</v>
+      </c>
+      <c r="C125" s="11">
+        <v>571910270</v>
+      </c>
+      <c r="D125" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="E125" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="F125" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B126" s="10">
+        <v>116</v>
+      </c>
+      <c r="C126" s="11">
+        <v>571910271</v>
+      </c>
+      <c r="D126" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="E126" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="F126" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B127" s="10">
+        <v>117</v>
+      </c>
+      <c r="C127" s="11">
+        <v>571910272</v>
+      </c>
+      <c r="D127" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="E127" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="F127" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B128" s="10">
+        <v>118</v>
+      </c>
+      <c r="C128" s="11">
+        <v>571910274</v>
+      </c>
+      <c r="D128" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="E128" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="F128" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B129" s="10">
+        <v>119</v>
+      </c>
+      <c r="C129" s="11">
+        <v>571910277</v>
+      </c>
+      <c r="D129" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="E129" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="F129" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B130" s="10">
+        <v>120</v>
+      </c>
+      <c r="C130" s="11">
+        <v>571910278</v>
+      </c>
+      <c r="D130" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="E130" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="F130" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B131" s="10">
+        <v>121</v>
+      </c>
+      <c r="C131" s="11">
+        <v>571910279</v>
+      </c>
+      <c r="D131" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="E131" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="F131" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B132" s="10">
+        <v>122</v>
+      </c>
+      <c r="C132" s="11">
+        <v>571910281</v>
+      </c>
+      <c r="D132" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="E132" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="F132" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B133" s="10">
+        <v>123</v>
+      </c>
+      <c r="C133" s="11">
+        <v>571910282</v>
+      </c>
+      <c r="D133" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="E133" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="F133" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B134" s="10">
+        <v>124</v>
+      </c>
+      <c r="C134" s="11">
+        <v>571910283</v>
+      </c>
+      <c r="D134" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="E134" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="F134" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B135" s="10">
+        <v>125</v>
+      </c>
+      <c r="C135" s="11">
+        <v>571910284</v>
+      </c>
+      <c r="D135" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="E135" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="F135" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B136" s="10">
+        <v>126</v>
+      </c>
+      <c r="C136" s="11">
+        <v>571910285</v>
+      </c>
+      <c r="D136" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="E136" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="F136" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B137" s="10">
+        <v>127</v>
+      </c>
+      <c r="C137" s="11">
+        <v>571910288</v>
+      </c>
+      <c r="D137" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="E137" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="F137" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B138" s="10">
+        <v>128</v>
+      </c>
+      <c r="C138" s="11">
+        <v>571910289</v>
+      </c>
+      <c r="D138" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="E138" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="F138" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B139" s="10">
+        <v>129</v>
+      </c>
+      <c r="C139" s="11">
+        <v>571910291</v>
+      </c>
+      <c r="D139" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="E139" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="F139" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B140" s="10">
+        <v>130</v>
+      </c>
+      <c r="C140" s="11">
+        <v>571910295</v>
+      </c>
+      <c r="D140" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="E140" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="F140" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B141" s="10">
+        <v>131</v>
+      </c>
+      <c r="C141" s="11">
+        <v>572010015</v>
+      </c>
+      <c r="D141" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="E141" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="F141" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" customHeight="1" ht="19.8">
+      <c r="B142" s="10">
+        <v>132</v>
+      </c>
+      <c r="C142" s="11">
+        <v>572010041</v>
+      </c>
+      <c r="D142" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="E142" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="F142" s="11" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2730,6 +3729,7 @@
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="D37:E37"/>
     <mergeCell ref="D73:E73"/>
+    <mergeCell ref="D109:E109"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.75" right="0.62" top="1" bottom="1.1" header="0.71" footer="0.5"/>

</xml_diff>